<commit_message>
Drew origin point for cultures
Need to turn the origin into regions by checking the suitability of the surrounding hexes.
</commit_message>
<xml_diff>
--- a/Planning/Troops.xlsx
+++ b/Planning/Troops.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Development\Unity Projects\Comitatus\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Documents\GitHub\Comitatus\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2732B67D-5E60-4051-9063-2910229FC749}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770B76D3-4011-438A-8864-D9EF88097162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="729" activeTab="3" xr2:uid="{D90EAD85-2583-4D9A-972D-2014937F672B}"/>
+    <workbookView xWindow="-24240" yWindow="1935" windowWidth="21600" windowHeight="11385" tabRatio="729" xr2:uid="{D90EAD85-2583-4D9A-972D-2014937F672B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cultures" sheetId="2" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Estuland</t>
   </si>
   <si>
-    <t>Steppe</t>
-  </si>
-  <si>
     <t>Related Terrain</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>WEAK</t>
+  </si>
+  <si>
+    <t>Desert/Dryland</t>
   </si>
 </sst>
 </file>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB0656D-050F-4AD8-9A1E-CDCC666E243C}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,16 +963,16 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,10 +980,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -994,13 +994,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1008,10 +1008,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1022,10 +1022,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -1039,7 +1039,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1047,16 +1047,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
         <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1095,31 +1095,31 @@
         <v>0</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>127</v>
-      </c>
       <c r="E1" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>122</v>
       </c>
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
@@ -1128,10 +1128,10 @@
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3">
         <v>7</v>
@@ -1156,10 +1156,10 @@
         <v>4</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
@@ -1196,18 +1196,18 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="3">
         <v>12</v>
@@ -1232,15 +1232,15 @@
         <v>4</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>2</v>
@@ -1268,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>3</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>2</v>
@@ -1304,15 +1304,15 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>2</v>
@@ -1340,15 +1340,15 @@
         <v>1</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>3</v>
@@ -1379,12 +1379,12 @@
         <v>2</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>3</v>
@@ -1415,12 +1415,12 @@
         <v>2</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>3</v>
@@ -1451,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1484,10 +1484,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1520,15 +1520,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>5</v>
@@ -1556,15 +1556,15 @@
         <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>5</v>
@@ -1592,10 +1592,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1640,310 +1640,310 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="L2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="M2" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="N2" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="I3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="K3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="L3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="8" t="s">
+      <c r="N3" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="I4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="L4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="H5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="8" t="s">
+      <c r="N5" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="L6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="M6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="F7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="J7" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="L7" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="K7" s="8" t="s">
+      <c r="N7" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECAC609-9966-4CDF-9687-3124F40B3B0C}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -2002,7 +2002,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>1</v>
@@ -2011,60 +2011,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>32</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="27" t="s">
         <v>33</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>34</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="28" t="s">
         <v>70</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="31"/>
       <c r="D2" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
       <c r="K2" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L2" s="34"/>
       <c r="M2" s="34"/>
@@ -2072,24 +2072,24 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
       <c r="D3" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="33"/>
       <c r="J3" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K3" s="33"/>
       <c r="L3" s="34"/>
@@ -2098,22 +2098,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
@@ -2124,51 +2124,51 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="32"/>
       <c r="G5" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K5" s="33"/>
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
       <c r="N5" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
@@ -2184,17 +2184,17 @@
       <c r="E7" s="31"/>
       <c r="F7" s="32"/>
       <c r="G7" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I7" s="33"/>
       <c r="J7" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>

</xml_diff>

<commit_message>
Faction culture assignments, autogen, divisional data collection
Regions now get assigned starting culture based on the regions' characteristics. Autogenerate func creates a new world every n seconds. Created data collection method to collect data needed for regional culture assignments.
</commit_message>
<xml_diff>
--- a/Planning/Troops.xlsx
+++ b/Planning/Troops.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Documents\GitHub\Comitatus\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770B76D3-4011-438A-8864-D9EF88097162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F066814-446D-4B44-865B-1335041833B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="1935" windowWidth="21600" windowHeight="11385" tabRatio="729" xr2:uid="{D90EAD85-2583-4D9A-972D-2014937F672B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="729" xr2:uid="{D90EAD85-2583-4D9A-972D-2014937F672B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cultures" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Troops Base Stats'!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -75,15 +77,6 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Cold</t>
-  </si>
-  <si>
-    <t>Hills</t>
-  </si>
-  <si>
-    <t>Woods</t>
-  </si>
-  <si>
     <t>Marsh</t>
   </si>
   <si>
@@ -342,9 +335,6 @@
     <t>Celtic</t>
   </si>
   <si>
-    <t>River</t>
-  </si>
-  <si>
     <t>Afon</t>
   </si>
   <si>
@@ -435,7 +425,19 @@
     <t>WEAK</t>
   </si>
   <si>
-    <t>Desert/Dryland</t>
+    <t>Taiga</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>Tundra</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Forest</t>
   </si>
 </sst>
 </file>
@@ -943,7 +945,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,16 +965,16 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,13 +982,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -994,13 +996,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1008,13 +1010,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1022,13 +1024,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1036,27 +1038,27 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1095,31 +1097,31 @@
         <v>0</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
@@ -1128,10 +1130,10 @@
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="3">
         <v>7</v>
@@ -1156,10 +1158,10 @@
         <v>4</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1168,10 +1170,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
@@ -1196,18 +1198,18 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C4" s="3">
         <v>12</v>
@@ -1232,15 +1234,15 @@
         <v>4</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>2</v>
@@ -1268,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>3</v>
@@ -1276,7 +1278,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>2</v>
@@ -1304,15 +1306,15 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>2</v>
@@ -1340,15 +1342,15 @@
         <v>1</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>3</v>
@@ -1379,12 +1381,12 @@
         <v>2</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>3</v>
@@ -1415,12 +1417,12 @@
         <v>2</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>3</v>
@@ -1451,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1484,10 +1486,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1520,15 +1522,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>5</v>
@@ -1556,15 +1558,15 @@
         <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>5</v>
@@ -1592,10 +1594,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1640,310 +1642,310 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="I1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="L2" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="M2" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="N2" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="L3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="M3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="M4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="N4" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="N5" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="H6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="K6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="L6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="M6" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="L7" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N7" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2002,7 +2004,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>1</v>
@@ -2011,60 +2013,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="31"/>
       <c r="D2" s="31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
       <c r="K2" s="33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L2" s="34"/>
       <c r="M2" s="34"/>
@@ -2072,24 +2074,24 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
       <c r="D3" s="31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I3" s="33"/>
       <c r="J3" s="33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K3" s="33"/>
       <c r="L3" s="34"/>
@@ -2098,22 +2100,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>127</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>131</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
@@ -2124,51 +2126,51 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="32"/>
       <c r="G5" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K5" s="33"/>
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
       <c r="N5" s="34" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="32" t="s">
         <v>127</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>131</v>
       </c>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
@@ -2176,7 +2178,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
@@ -2184,17 +2186,17 @@
       <c r="E7" s="31"/>
       <c r="F7" s="32"/>
       <c r="G7" s="32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I7" s="33"/>
       <c r="J7" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>

</xml_diff>